<commit_message>
Added google API support
</commit_message>
<xml_diff>
--- a/data/penalty_log.xlsx
+++ b/data/penalty_log.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L462"/>
+  <dimension ref="A1:L476"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F50" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
@@ -20860,8 +20860,6 @@
           <t>furkhang.552</t>
         </is>
       </c>
-      <c r="C462" t="inlineStr"/>
-      <c r="D462" t="inlineStr"/>
       <c r="E462" t="inlineStr">
         <is>
           <t>JL</t>
@@ -20870,13 +20868,11 @@
       <c r="F462" t="n">
         <v>10</v>
       </c>
-      <c r="G462" t="inlineStr"/>
       <c r="H462" t="inlineStr">
         <is>
           <t>https://www.youtube.com/watch?v=6q8f39GldsQ&amp;ab_channel=DeuxMachina&amp;t=90</t>
         </is>
       </c>
-      <c r="I462" t="inlineStr"/>
       <c r="J462" t="inlineStr">
         <is>
           <t>juan64</t>
@@ -20890,7 +20886,621 @@
         </is>
       </c>
       <c r="L462" s="2" t="n">
-        <v>45281.72770226347</v>
+        <v>45281.72770226852</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>6359</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="E463" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="F463" t="n">
+        <v>3</v>
+      </c>
+      <c r="H463" t="inlineStr">
+        <is>
+          <t>https://youtu.be/&amp;t=3525</t>
+        </is>
+      </c>
+      <c r="J463" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="K463" t="inlineStr">
+        <is>
+          <t>edfvswfv</t>
+        </is>
+      </c>
+      <c r="L463" s="2" t="n">
+        <v>45310.00884177083</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>6359</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>fgnhfgnh</t>
+        </is>
+      </c>
+      <c r="D464" t="inlineStr">
+        <is>
+          <t>dhbfth</t>
+        </is>
+      </c>
+      <c r="E464" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="F464" t="n">
+        <v>3</v>
+      </c>
+      <c r="G464" t="inlineStr">
+        <is>
+          <t>Edging/Bumping/Swerving on Straights</t>
+        </is>
+      </c>
+      <c r="H464" t="inlineStr">
+        <is>
+          <t>https://youtu.be/&amp;t=3525</t>
+        </is>
+      </c>
+      <c r="I464" t="inlineStr">
+        <is>
+          <t>dhttdrh</t>
+        </is>
+      </c>
+      <c r="J464" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="K464" t="inlineStr">
+        <is>
+          <t>edfvswfv</t>
+        </is>
+      </c>
+      <c r="L464" s="2" t="n">
+        <v>45310.00884177083</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>9884</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="E465" t="inlineStr">
+        <is>
+          <t>UL</t>
+        </is>
+      </c>
+      <c r="F465" t="n">
+        <v>3</v>
+      </c>
+      <c r="H465" t="inlineStr">
+        <is>
+          <t>https://youtu.be/&amp;t=234</t>
+        </is>
+      </c>
+      <c r="J465" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="K465" t="inlineStr">
+        <is>
+          <t>eafvf</t>
+        </is>
+      </c>
+      <c r="L465" s="2" t="n">
+        <v>45310.0130899537</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>9884</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>No offence</t>
+        </is>
+      </c>
+      <c r="E466" t="inlineStr">
+        <is>
+          <t>UL</t>
+        </is>
+      </c>
+      <c r="F466" t="n">
+        <v>3</v>
+      </c>
+      <c r="H466" t="inlineStr">
+        <is>
+          <t>https://youtu.be/&amp;t=234</t>
+        </is>
+      </c>
+      <c r="I466" t="inlineStr">
+        <is>
+          <t>rdgdr</t>
+        </is>
+      </c>
+      <c r="J466" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="K466" t="inlineStr">
+        <is>
+          <t>eafvf</t>
+        </is>
+      </c>
+      <c r="L466" s="2" t="n">
+        <v>45310.0130899537</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>6437</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="E467" t="inlineStr">
+        <is>
+          <t>UL</t>
+        </is>
+      </c>
+      <c r="F467" t="n">
+        <v>5</v>
+      </c>
+      <c r="H467" t="inlineStr">
+        <is>
+          <t>https://youtu.be/&amp;t=352</t>
+        </is>
+      </c>
+      <c r="J467" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="K467" t="inlineStr">
+        <is>
+          <t>gvsrgv</t>
+        </is>
+      </c>
+      <c r="L467" s="2" t="n">
+        <v>45310.01524820602</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>6437</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>No offence</t>
+        </is>
+      </c>
+      <c r="E468" t="inlineStr">
+        <is>
+          <t>UL</t>
+        </is>
+      </c>
+      <c r="F468" t="n">
+        <v>5</v>
+      </c>
+      <c r="H468" t="inlineStr">
+        <is>
+          <t>https://youtu.be/&amp;t=352</t>
+        </is>
+      </c>
+      <c r="I468" t="inlineStr">
+        <is>
+          <t>rhbtrb</t>
+        </is>
+      </c>
+      <c r="J468" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="K468" t="inlineStr">
+        <is>
+          <t>gvsrgv</t>
+        </is>
+      </c>
+      <c r="L468" s="2" t="n">
+        <v>45310.01524820602</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>5446</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="E469" t="inlineStr">
+        <is>
+          <t>UL</t>
+        </is>
+      </c>
+      <c r="F469" t="n">
+        <v>3</v>
+      </c>
+      <c r="H469" t="inlineStr">
+        <is>
+          <t>https://youtu.be/&amp;t=352</t>
+        </is>
+      </c>
+      <c r="J469" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="K469" t="inlineStr">
+        <is>
+          <t>edgfw</t>
+        </is>
+      </c>
+      <c r="L469" s="2" t="n">
+        <v>45310.01578501157</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>5446</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>No offence</t>
+        </is>
+      </c>
+      <c r="E470" t="inlineStr">
+        <is>
+          <t>UL</t>
+        </is>
+      </c>
+      <c r="F470" t="n">
+        <v>3</v>
+      </c>
+      <c r="H470" t="inlineStr">
+        <is>
+          <t>https://youtu.be/&amp;t=352</t>
+        </is>
+      </c>
+      <c r="I470" t="inlineStr">
+        <is>
+          <t>fvdsvs</t>
+        </is>
+      </c>
+      <c r="J470" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="K470" t="inlineStr">
+        <is>
+          <t>edgfw</t>
+        </is>
+      </c>
+      <c r="L470" s="2" t="n">
+        <v>45310.01578501157</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>3925</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="E471" t="inlineStr">
+        <is>
+          <t>UL</t>
+        </is>
+      </c>
+      <c r="F471" t="n">
+        <v>4</v>
+      </c>
+      <c r="H471" t="inlineStr">
+        <is>
+          <t>https://youtu.be/&amp;t=352</t>
+        </is>
+      </c>
+      <c r="J471" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="K471" t="inlineStr">
+        <is>
+          <t>dafvadsv</t>
+        </is>
+      </c>
+      <c r="L471" s="2" t="n">
+        <v>45310.01768652778</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>3925</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>No offence</t>
+        </is>
+      </c>
+      <c r="E472" t="inlineStr">
+        <is>
+          <t>UL</t>
+        </is>
+      </c>
+      <c r="F472" t="n">
+        <v>4</v>
+      </c>
+      <c r="H472" t="inlineStr">
+        <is>
+          <t>https://youtu.be/&amp;t=352</t>
+        </is>
+      </c>
+      <c r="I472" t="inlineStr">
+        <is>
+          <t>afcsdv</t>
+        </is>
+      </c>
+      <c r="J472" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="K472" t="inlineStr">
+        <is>
+          <t>dafvadsv</t>
+        </is>
+      </c>
+      <c r="L472" s="2" t="n">
+        <v>45310.01768652778</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>6747</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="E473" t="inlineStr">
+        <is>
+          <t>UL</t>
+        </is>
+      </c>
+      <c r="F473" t="n">
+        <v>4</v>
+      </c>
+      <c r="H473" t="inlineStr">
+        <is>
+          <t>https://youtu.be/&amp;t=352</t>
+        </is>
+      </c>
+      <c r="J473" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="K473" t="inlineStr">
+        <is>
+          <t>svdrg</t>
+        </is>
+      </c>
+      <c r="L473" s="2" t="n">
+        <v>45310.02423076389</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>6747</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>No offence</t>
+        </is>
+      </c>
+      <c r="E474" t="inlineStr">
+        <is>
+          <t>UL</t>
+        </is>
+      </c>
+      <c r="F474" t="n">
+        <v>4</v>
+      </c>
+      <c r="H474" t="inlineStr">
+        <is>
+          <t>https://youtu.be/&amp;t=352</t>
+        </is>
+      </c>
+      <c r="I474" t="inlineStr">
+        <is>
+          <t>fgdrg</t>
+        </is>
+      </c>
+      <c r="J474" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="K474" t="inlineStr">
+        <is>
+          <t>svdrg</t>
+        </is>
+      </c>
+      <c r="L474" s="2" t="n">
+        <v>45310.02423076389</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>2171</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="E475" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="F475" t="n">
+        <v>4</v>
+      </c>
+      <c r="H475" t="inlineStr">
+        <is>
+          <t>https://youtu.be/&amp;t=352</t>
+        </is>
+      </c>
+      <c r="J475" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="K475" t="inlineStr">
+        <is>
+          <t>wesgvswgv</t>
+        </is>
+      </c>
+      <c r="L475" s="2" t="n">
+        <v>45310.02582716435</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>2171</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>No offence</t>
+        </is>
+      </c>
+      <c r="D476" t="inlineStr"/>
+      <c r="E476" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="F476" t="n">
+        <v>4</v>
+      </c>
+      <c r="G476" t="inlineStr"/>
+      <c r="H476" t="inlineStr">
+        <is>
+          <t>https://youtu.be/&amp;t=352</t>
+        </is>
+      </c>
+      <c r="I476" t="inlineStr">
+        <is>
+          <t>dasvfds</t>
+        </is>
+      </c>
+      <c r="J476" t="inlineStr">
+        <is>
+          <t>_gorlomi</t>
+        </is>
+      </c>
+      <c r="K476" t="inlineStr">
+        <is>
+          <t>wesgvswgv</t>
+        </is>
+      </c>
+      <c r="L476" s="2" t="n">
+        <v>45310.02582716673</v>
       </c>
     </row>
   </sheetData>

</xml_diff>